<commit_message>
update ignore file list
</commit_message>
<xml_diff>
--- a/Upload/FundClientTrades.xlsx
+++ b/Upload/FundClientTrades.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="163">
   <si>
     <t>Portfolio Name</t>
   </si>
@@ -1603,8 +1603,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F1060" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F1060"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F1066" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F1066"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Portfolio Name"/>
     <tableColumn id="2" name="Security ID" dataDxfId="3"/>
@@ -1904,11 +1904,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1047667"/>
+  <dimension ref="A1:J1047665"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1031" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1053" sqref="A1053:A1060"/>
+      <pane ySplit="1" topLeftCell="A1028" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1062" sqref="I1062"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24131,7 +24131,127 @@
         <v>20180207</v>
       </c>
     </row>
-    <row r="1047667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1061" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1061" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1061" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1061" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1061" s="41">
+        <v>700</v>
+      </c>
+      <c r="E1061" s="41">
+        <v>18.36542857142857</v>
+      </c>
+      <c r="F1061">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1062" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1062" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1062" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1062" s="41">
+        <v>3000</v>
+      </c>
+      <c r="E1062" s="41">
+        <v>67.718976666666663</v>
+      </c>
+      <c r="F1062">
+        <v>20180306</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1063" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1063" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1063" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1063" s="41">
+        <v>11</v>
+      </c>
+      <c r="E1063" s="41">
+        <v>371.5</v>
+      </c>
+      <c r="F1063" s="47">
+        <v>20180306</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1064" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1064" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1064" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1064" s="41">
+        <v>700</v>
+      </c>
+      <c r="E1064" s="41">
+        <v>18.36542857142857</v>
+      </c>
+      <c r="F1064" s="47">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1065" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1065" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1065" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1065" s="41">
+        <v>3000</v>
+      </c>
+      <c r="E1065" s="41">
+        <v>67.718976666666663</v>
+      </c>
+      <c r="F1065" s="47">
+        <v>20180306</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1066" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1066" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1066" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1066" s="41">
+        <v>11</v>
+      </c>
+      <c r="E1066" s="41">
+        <v>371.5</v>
+      </c>
+      <c r="F1066" s="47">
+        <v>20180306</v>
+      </c>
+    </row>
+    <row r="1047665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>